<commit_message>
Tested terminals and updated scripts
</commit_message>
<xml_diff>
--- a/SeattleTerminal46/Test.xlsx
+++ b/SeattleTerminal46/Test.xlsx
@@ -1,13 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Blume-proj\PortTerminalScraping\SeattleTerminal46\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7260"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId3" sheetId="1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -371,11 +378,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -387,7 +393,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -405,18 +411,294 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:H30"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -436,7 +718,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -456,7 +738,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -476,7 +758,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -496,7 +778,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -516,7 +798,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -536,7 +818,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -556,7 +838,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -576,7 +858,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -596,7 +878,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -616,7 +898,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -636,7 +918,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -656,7 +938,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -676,7 +958,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -696,7 +978,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>63</v>
       </c>
@@ -716,7 +998,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -736,7 +1018,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -756,7 +1038,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>73</v>
       </c>
@@ -776,7 +1058,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>78</v>
       </c>
@@ -796,7 +1078,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>82</v>
       </c>
@@ -816,7 +1098,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>87</v>
       </c>
@@ -836,7 +1118,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>90</v>
       </c>
@@ -856,7 +1138,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>94</v>
       </c>
@@ -876,7 +1158,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>97</v>
       </c>
@@ -896,7 +1178,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>100</v>
       </c>
@@ -916,7 +1198,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>103</v>
       </c>
@@ -936,7 +1218,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>106</v>
       </c>
@@ -956,7 +1238,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>109</v>
       </c>
@@ -976,7 +1258,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>113</v>
       </c>
@@ -996,7 +1278,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>116</v>
       </c>
@@ -1017,6 +1299,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>